<commit_message>
- testdata en datasets toegevoegd - weergave concepten aangepast
</commit_message>
<xml_diff>
--- a/catalogusdata/Testdata DSO.xlsx
+++ b/catalogusdata/Testdata DSO.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\lwortel\Documents\Klussen\Kadaster\Deliveries\Dataimport\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\data\ith21266\Documents\Kadaster\bp4mc2\catalogusdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12132" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="kenniskluis" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
   <si>
     <t>Uploadcontainer</t>
   </si>
@@ -108,6 +109,33 @@
   </si>
   <si>
     <t>Registraties &gt; BAG</t>
+  </si>
+  <si>
+    <t>Upload concepten (RDF of Turtle)</t>
+  </si>
+  <si>
+    <t>Upload status (RDF of Turtle)</t>
+  </si>
+  <si>
+    <t>status.ttl</t>
+  </si>
+  <si>
+    <t>Upload een enkel concept (RDF of Turtle)</t>
+  </si>
+  <si>
+    <t>Beheer -&gt; Rapportages -&gt; Missing Links
+Beheer -&gt; Rapportages -&gt; Statuscontrole</t>
+  </si>
+  <si>
+    <t>Hoofdpagina -&gt; toon alles 
+Begripspagina (klik op bv hond)
+Beheer -&gt; Rapportages -&gt; Relatiecontrole
+Beheer -&gt; Rapportages -&gt; Missing Links
+Beheer -&gt; Rapportages -&gt; Statuscontrole
+Beheer -&gt; Rapportages -&gt; Looping</t>
+  </si>
+  <si>
+    <t>testdata kenniskluis.ttl</t>
   </si>
 </sst>
 </file>
@@ -159,7 +187,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -175,9 +203,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Kantoor">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -215,7 +243,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Kantoor">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -287,7 +315,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Kantoor">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -439,19 +467,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="45.42578125" customWidth="1"/>
+    <col min="1" max="1" width="45.44140625" customWidth="1"/>
     <col min="2" max="2" width="34" customWidth="1"/>
-    <col min="3" max="3" width="51.28515625" customWidth="1"/>
-    <col min="4" max="4" width="46.7109375" customWidth="1"/>
+    <col min="3" max="3" width="51.33203125" customWidth="1"/>
+    <col min="4" max="4" width="46.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -465,7 +493,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -476,7 +504,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -487,7 +515,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -498,7 +526,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -509,7 +537,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -520,7 +548,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -534,7 +562,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -547,6 +575,89 @@
       <c r="D8" s="2" t="s">
         <v>24</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="45.44140625" customWidth="1"/>
+    <col min="2" max="2" width="34" customWidth="1"/>
+    <col min="3" max="3" width="51.33203125" customWidth="1"/>
+    <col min="4" max="4" width="46.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>